<commit_message>
VERSION 3.0: FINALIZADO (documentando)
</commit_message>
<xml_diff>
--- a/estructura/estructura.xlsx
+++ b/estructura/estructura.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juang\Informatica\2DAM\Interfaz\ImportadorProductos\estructura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859CE507-F12D-4BF7-B5E2-195FDB8D06D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345A5504-0F50-48A0-8718-4DEDF9CF1E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2393" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2427" uniqueCount="876">
   <si>
     <t>CODIGO</t>
   </si>
@@ -7602,6 +7602,57 @@
   </si>
   <si>
     <t>TARIFA 2</t>
+  </si>
+  <si>
+    <t>ALMACEN PRINCIPAL</t>
+  </si>
+  <si>
+    <t>ALMACEN.NOMBRE.1</t>
+  </si>
+  <si>
+    <t>ALMACEN.NOMBRE.2</t>
+  </si>
+  <si>
+    <t>ALMACEN.NOMBRE.3</t>
+  </si>
+  <si>
+    <t>ALMACEN 2</t>
+  </si>
+  <si>
+    <t>STOCKS.CODIGO_ALMACEN.1</t>
+  </si>
+  <si>
+    <t>STOCKS.CODIGO_ALMACEN.2</t>
+  </si>
+  <si>
+    <t>STOCKS.CODIGO_ALMACEN.3</t>
+  </si>
+  <si>
+    <t>ALMACEN 3</t>
+  </si>
+  <si>
+    <t>ALMACEN</t>
+  </si>
+  <si>
+    <t>STOCKS.CODIGO_ARTICULO.1</t>
+  </si>
+  <si>
+    <t>STOCKS.CODIGO_ARTICULO.2</t>
+  </si>
+  <si>
+    <t>STOCKS.CODIGO_ARTICULO.3</t>
+  </si>
+  <si>
+    <t>ARTICULO.STOCK</t>
+  </si>
+  <si>
+    <t>STOCKS.STOCK.1</t>
+  </si>
+  <si>
+    <t>STOCKS.STOCK.2</t>
+  </si>
+  <si>
+    <t>STOCKS.STOCK.3</t>
   </si>
 </sst>
 </file>
@@ -7685,7 +7736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7731,6 +7782,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8066,10 +8120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B87C35E-C910-4037-AD71-C165640BA7DE}">
-  <dimension ref="A1:AN7"/>
+  <dimension ref="A1:BA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AN8" sqref="AN8"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AW16" sqref="AW16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8082,67 +8136,78 @@
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="23" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="25.5546875" customWidth="1"/>
+    <col min="47" max="47" width="15" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="25.5546875" customWidth="1"/>
+    <col min="50" max="50" width="15" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
       <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>8</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>8</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
       <c r="G2" t="s">
         <v>822</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>841</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>843</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>856</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>814</v>
       </c>
@@ -8155,56 +8220,74 @@
       <c r="G3" t="s">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>2</v>
       </c>
-      <c r="K3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="L3" t="s">
         <v>1</v>
       </c>
       <c r="O3" t="s">
         <v>1</v>
       </c>
-      <c r="T3" t="s">
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
         <v>2</v>
       </c>
-      <c r="U3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y3" t="s">
+      <c r="V3" t="s">
         <v>1</v>
       </c>
       <c r="Z3" t="s">
         <v>1</v>
       </c>
       <c r="AA3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="s">
         <v>2</v>
       </c>
-      <c r="AB3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF3" t="s">
+      <c r="AC3" t="s">
         <v>1</v>
       </c>
       <c r="AG3" t="s">
         <v>1</v>
       </c>
       <c r="AH3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI3" t="s">
         <v>2</v>
       </c>
-      <c r="AI3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM3" t="s">
+      <c r="AJ3" t="s">
         <v>1</v>
       </c>
       <c r="AN3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>0</v>
       </c>
@@ -8217,25 +8300,22 @@
       <c r="G4" t="s">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
-        <v>0</v>
-      </c>
       <c r="K4" t="s">
         <v>0</v>
       </c>
-      <c r="N4" t="s">
+      <c r="L4" t="s">
         <v>0</v>
       </c>
       <c r="O4" t="s">
         <v>0</v>
       </c>
-      <c r="T4" t="s">
+      <c r="P4" t="s">
         <v>0</v>
       </c>
       <c r="U4" t="s">
         <v>0</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="V4" t="s">
         <v>0</v>
       </c>
       <c r="Z4" t="s">
@@ -8247,7 +8327,7 @@
       <c r="AB4" t="s">
         <v>0</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AC4" t="s">
         <v>0</v>
       </c>
       <c r="AG4" t="s">
@@ -8259,14 +8339,35 @@
       <c r="AI4" t="s">
         <v>0</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AJ4" t="s">
         <v>0</v>
       </c>
       <c r="AN4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>813</v>
       </c>
@@ -8279,56 +8380,74 @@
       <c r="G5" t="s">
         <v>4</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>13</v>
       </c>
-      <c r="K5" t="s">
-        <v>793</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="L5" t="s">
         <v>793</v>
       </c>
       <c r="O5" t="s">
         <v>793</v>
       </c>
-      <c r="T5" t="s">
+      <c r="P5" t="s">
+        <v>793</v>
+      </c>
+      <c r="U5" t="s">
         <v>13</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>810</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>3</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>4</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>13</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>810</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>3</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>4</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>13</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>810</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AN5" t="s">
         <v>3</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AS5" t="s">
+        <v>868</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>868</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>868</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>817</v>
       </c>
@@ -8354,186 +8473,280 @@
         <v>824</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>826</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>831</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>833</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>834</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>835</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>836</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="W6" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>839</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>840</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Z6" s="1" t="s">
         <v>841</v>
       </c>
-      <c r="Z6" s="1" t="s">
+      <c r="AA6" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
         <v>844</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AC6" s="1" t="s">
         <v>846</v>
       </c>
-      <c r="AC6" s="1" t="s">
+      <c r="AD6" s="1" t="s">
         <v>847</v>
       </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AE6" s="1" t="s">
         <v>848</v>
       </c>
-      <c r="AE6" s="1" t="s">
+      <c r="AF6" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="AF6" s="1" t="s">
+      <c r="AG6" s="1" t="s">
         <v>843</v>
       </c>
-      <c r="AG6" s="1" t="s">
+      <c r="AH6" s="1" t="s">
         <v>850</v>
       </c>
-      <c r="AH6" s="1" t="s">
+      <c r="AI6" s="1" t="s">
         <v>852</v>
       </c>
-      <c r="AI6" s="1" t="s">
+      <c r="AJ6" s="1" t="s">
         <v>845</v>
       </c>
-      <c r="AJ6" s="1" t="s">
+      <c r="AK6" s="1" t="s">
         <v>853</v>
       </c>
-      <c r="AK6" s="1" t="s">
+      <c r="AL6" s="1" t="s">
         <v>854</v>
       </c>
-      <c r="AL6" s="1" t="s">
+      <c r="AM6" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="AM6" s="1" t="s">
+      <c r="AN6" s="1" t="s">
         <v>856</v>
       </c>
-      <c r="AN6" s="1" t="s">
+      <c r="AO6" s="1" t="s">
         <v>857</v>
       </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AP6" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="AQ6" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="AR6" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="AS6" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="AT6" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="AU6" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="AV6" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="AW6" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="AX6" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="AY6" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="AZ6" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="BA6" s="1" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
       <c r="H7" s="17"/>
-      <c r="J7" s="2" t="str">
+      <c r="I7" s="17"/>
+      <c r="K7" s="2" t="str">
         <f>IF(ISBLANK(A7),"",A7)</f>
         <v/>
       </c>
-      <c r="K7" t="str">
-        <f>IF(ISBLANK(I7),"",I7)</f>
+      <c r="L7" t="str">
+        <f>IF(ISBLANK(J7),"",J7)</f>
         <v/>
       </c>
-      <c r="M7" s="12"/>
-      <c r="N7" t="str">
-        <f>IF(ISBLANK(I7),"",I7)</f>
+      <c r="N7" s="12"/>
+      <c r="O7" t="str">
+        <f>IF(ISBLANK(J7),"",J7)</f>
         <v/>
       </c>
-      <c r="O7" t="str">
-        <f>IF(ISBLANK(I7),"",I7)</f>
+      <c r="P7" t="str">
+        <f>IF(ISBLANK(J7),"",J7)</f>
         <v/>
       </c>
-      <c r="S7" t="str">
-        <f>IF(ISBLANK(I7),"",I7)</f>
+      <c r="T7" t="str">
+        <f>IF(ISBLANK(J7),"",J7)</f>
         <v/>
       </c>
-      <c r="T7" s="2" t="str">
+      <c r="U7" s="2" t="str">
         <f>IF(ISBLANK(A7),"",A7)</f>
         <v/>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>809</v>
       </c>
-      <c r="W7" s="13">
-        <f>V7/(E7*0.01+1)</f>
-        <v>0</v>
-      </c>
-      <c r="X7" s="14"/>
-      <c r="Y7" t="str">
+      <c r="X7" s="13">
+        <f>W7/(E7*0.01+1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="18">
+        <f>X7*0.1</f>
+        <v>0</v>
+      </c>
+      <c r="Z7" t="str">
         <f>IF(ISBLANK(F7),"",F7)</f>
         <v/>
       </c>
-      <c r="Z7" t="str">
+      <c r="AA7" t="str">
         <f>IF(ISBLANK(G7),"",G7)</f>
         <v/>
       </c>
-      <c r="AA7" s="2" t="str">
+      <c r="AB7" s="2" t="str">
         <f>IF(ISBLANK(A7),"",A7)</f>
         <v/>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>851</v>
       </c>
-      <c r="AD7" s="13">
-        <f>AC7/(E7*0.01+1)</f>
-        <v>0</v>
-      </c>
-      <c r="AE7" s="14"/>
-      <c r="AF7" t="str">
+      <c r="AE7" s="13">
+        <f>AD7/(E7*0.01+1)</f>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="18">
+        <f>AE7*0.1</f>
+        <v>0</v>
+      </c>
+      <c r="AG7" t="str">
         <f>IF(ISBLANK(F7),"",F7)</f>
         <v/>
       </c>
-      <c r="AG7" t="str">
+      <c r="AH7" t="str">
         <f>IF(ISBLANK(G7),"",G7)</f>
         <v/>
       </c>
-      <c r="AH7" s="2" t="str">
+      <c r="AI7" s="2" t="str">
         <f>IF(ISBLANK(A7),"",A7)</f>
         <v/>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>858</v>
       </c>
-      <c r="AK7" s="13">
-        <f>AJ7/(E7*0.01+1)</f>
-        <v>0</v>
-      </c>
-      <c r="AL7" s="14"/>
-      <c r="AM7" t="str">
+      <c r="AL7" s="13">
+        <f>AK7/(E7*0.01+1)</f>
+        <v>0</v>
+      </c>
+      <c r="AM7" s="18">
+        <f>AL7*0.1</f>
+        <v>0</v>
+      </c>
+      <c r="AN7" t="str">
         <f>IF(ISBLANK(F7),"",F7)</f>
         <v/>
       </c>
-      <c r="AN7" t="str">
+      <c r="AO7" t="str">
         <f>IF(ISBLANK(G7),"",G7)</f>
+        <v/>
+      </c>
+      <c r="AP7" t="s">
+        <v>859</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>863</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>867</v>
+      </c>
+      <c r="AS7" t="str">
+        <f>AP7</f>
+        <v>ALMACEN PRINCIPAL</v>
+      </c>
+      <c r="AT7" t="str">
+        <f>IF(ISBLANK(A7),"",A7)</f>
+        <v/>
+      </c>
+      <c r="AU7" t="str">
+        <f>IF(ISBLANK($I7),"",$I7)</f>
+        <v/>
+      </c>
+      <c r="AV7" t="str">
+        <f>AQ7</f>
+        <v>ALMACEN 2</v>
+      </c>
+      <c r="AW7" t="str">
+        <f>IF(ISBLANK(A7),"",A7)</f>
+        <v/>
+      </c>
+      <c r="AX7" t="str">
+        <f>IF(ISBLANK($I7),"",$I7)</f>
+        <v/>
+      </c>
+      <c r="AY7" t="str">
+        <f>AR7</f>
+        <v>ALMACEN 3</v>
+      </c>
+      <c r="AZ7" t="str">
+        <f>IF(ISBLANK(A7),"",A7)</f>
+        <v/>
+      </c>
+      <c r="BA7" t="str">
+        <f>IF(ISBLANK($I7),"",$I7)</f>
         <v/>
       </c>
     </row>

</xml_diff>